<commit_message>
Cambiato modo di calcolare i valori medi per ecosistemi (approvvigionamento). Ora la media pesata avviene sui valori di eco_contribution per classe corine. I pesi sono le superfici corine. Se le superfici corine sono zero per una determinata classe, il contributo è posto uguale a zero (es. risaie in Umbria)
</commit_message>
<xml_diff>
--- a/data-raw/elenco.xlsx
+++ b/data-raw/elenco.xlsx
@@ -1,18 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rsericerca-my.sharepoint.com/personal/mela_rse-web_it/Documents/R/miei_pacchetti/ecoservr/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_DE08F77FC3574AFC124848B51A6D72CD2EF1F2A0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39A10AD5-16FD-479B-BD6A-B63A2030864D}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView minimized="1" xWindow="2835" yWindow="1080" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>x</t>
   </si>
@@ -489,16 +509,33 @@
   </si>
   <si>
     <t>altri beni e servizi: Sifim</t>
+  </si>
+  <si>
+    <t>valori</t>
+  </si>
+  <si>
+    <t>pesi superfici</t>
+  </si>
+  <si>
+    <t>eco con</t>
+  </si>
+  <si>
+    <t>controbution</t>
+  </si>
+  <si>
+    <t>media ponderata valori unitari</t>
+  </si>
+  <si>
+    <t>media ponderata eco con</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -510,7 +547,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -528,24 +565,331 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -553,7 +897,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,7 +905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -569,7 +913,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -577,7 +921,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -585,7 +929,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -593,7 +937,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -601,7 +945,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -609,7 +953,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -617,7 +961,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -625,7 +969,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -633,7 +977,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -641,7 +985,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -649,7 +993,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -657,7 +1001,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -665,7 +1009,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -673,7 +1017,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -681,7 +1025,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -689,7 +1033,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -697,7 +1041,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -705,7 +1049,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -713,7 +1057,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -721,7 +1065,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -729,7 +1073,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -737,7 +1081,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -745,7 +1089,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -753,7 +1097,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -761,7 +1105,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -769,7 +1113,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -777,7 +1121,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -785,7 +1129,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -793,7 +1137,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -801,7 +1145,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -809,7 +1153,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -817,7 +1161,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -825,7 +1169,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -833,7 +1177,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -841,7 +1185,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -849,7 +1193,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -857,7 +1201,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -865,7 +1209,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -873,7 +1217,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -881,7 +1225,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -889,7 +1233,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -897,7 +1241,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -905,7 +1249,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -913,7 +1257,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -921,7 +1265,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -929,7 +1273,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -937,7 +1281,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -945,7 +1289,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -953,7 +1297,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -961,7 +1305,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -969,7 +1313,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -977,7 +1321,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -985,7 +1329,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -993,7 +1337,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1001,7 +1345,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1009,7 +1353,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1017,7 +1361,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1025,7 +1369,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1033,7 +1377,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1041,7 +1385,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1049,7 +1393,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1057,7 +1401,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1065,7 +1409,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1073,7 +1417,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1081,7 +1425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1089,7 +1433,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1097,7 +1441,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1105,7 +1449,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1113,7 +1457,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1121,7 +1465,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1129,7 +1473,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1137,7 +1481,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1145,7 +1489,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1153,7 +1497,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1161,7 +1505,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1169,7 +1513,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1178,6 +1522,121 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E199F60-5E97-4DD5-A872-4705078A8EC9}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>30</v>
+      </c>
+      <c r="B1">
+        <v>45</v>
+      </c>
+      <c r="C1">
+        <v>60</v>
+      </c>
+      <c r="D1">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>59</v>
+      </c>
+      <c r="D2">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>0.36</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>+A1*A3</f>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:D5" si="0">+B1*B3</f>
+        <v>16.2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G5">
+        <f>+AVERAGE(A5:D5)</f>
+        <v>9.6750000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>+SUMPRODUCT(A1:D1,A2:D2)/SUM(A2:D2)</f>
+        <v>59.210526315789473</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="array" ref="A8">+SUMPRODUCT(A3:D3,A2:D2)/SUM(A2:D2)</f>
+        <v>0.15098684210526314</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>+A7*A8</f>
+        <v>8.9400103878116326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>